<commit_message>
Refactoring : Algorithme 1
</commit_message>
<xml_diff>
--- a/TP2 Search/TP2 Complexity.xlsx
+++ b/TP2 Search/TP2 Complexity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Barhouch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IL\complexity\advanced-algorithmics-and-complexity\TP2 Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C09212-4664-4D19-BB52-F3732951A3EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBFF7A8-68E5-4B98-A912-F803B63521D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16D324BE-EF6A-412D-8845-EBC60A736D46}"/>
   </bookViews>
@@ -1335,28 +1335,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.01</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1452,31 +1452,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9.9999999999999699E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.999990000099993E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9999700002999851E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9999500004999772E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9999300006999684E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1999890001099953E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3999870001299946E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5999850001499939E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.799983000169993E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1527,8 +1527,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2058,8 +2059,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2413,7 +2415,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2509,31 +2511,31 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7.9932568819676459E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4744988988716072E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9557409157755685E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2372494494358031E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.4369829326795308E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7184914663397644E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.8255160437278719E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9182249495834932E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2584,8 +2586,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3115,8 +3118,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3566,31 +3570,31 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0000000000000002E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7999999999999999E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3686,31 +3690,31 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8.0000000000000004E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.4999999999999995E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9999999999999998E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2000000000000003E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3999999999999997E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7000000000000005E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.7999999999999997E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.8999999999999999E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3761,8 +3765,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -8201,16 +8206,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8537,8 +8542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AFFE7-F229-43C6-BA9F-9CAF56C460D3}">
   <dimension ref="B3:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M51" sqref="M51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8779,8 +8784,8 @@
       <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="2">
-        <v>2.4999750002499901E-9</v>
+      <c r="C19" s="3">
+        <v>0</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -8817,8 +8822,8 @@
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f xml:space="preserve"> (4*B22 + 4)*C19</f>
-        <v>9.9999999999999699E-4</v>
+        <f xml:space="preserve"> (6*B22 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <v>100000</v>
@@ -8836,11 +8841,11 @@
         <v>200000</v>
       </c>
       <c r="C23" s="1">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1">
-        <f xml:space="preserve"> (4*B23 + 4)*C19</f>
-        <v>1.999990000099993E-3</v>
+        <f xml:space="preserve"> (6*B23 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <v>200000</v>
@@ -8858,11 +8863,11 @@
         <v>400000</v>
       </c>
       <c r="C24" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1">
-        <f xml:space="preserve"> (4*B24 + 4)*C19</f>
-        <v>3.9999700002999851E-3</v>
+        <f xml:space="preserve"> (6*B24 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
         <v>400000</v>
@@ -8880,11 +8885,11 @@
         <v>600000</v>
       </c>
       <c r="C25" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1">
-        <f xml:space="preserve"> (4*B25 + 4)*C19</f>
-        <v>5.9999500004999772E-3</v>
+        <f xml:space="preserve"> (6*B25 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
         <v>600000</v>
@@ -8902,11 +8907,11 @@
         <v>800000</v>
       </c>
       <c r="C26" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
-        <f xml:space="preserve"> (4*B26 + 4)*C19</f>
-        <v>7.9999300006999684E-3</v>
+        <f xml:space="preserve"> (6*B26 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F26" s="4">
         <v>800000</v>
@@ -8924,11 +8929,11 @@
         <v>1200000</v>
       </c>
       <c r="C27" s="1">
-        <v>7.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="D27" s="1">
-        <f xml:space="preserve"> (4*B27 + 4)*C19</f>
-        <v>1.1999890001099953E-2</v>
+        <f xml:space="preserve"> (6*B27 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
         <v>1200000</v>
@@ -8946,11 +8951,11 @@
         <v>1400000</v>
       </c>
       <c r="C28" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D28" s="1">
-        <f xml:space="preserve"> (4*B28 + 4)*C19</f>
-        <v>1.3999870001299946E-2</v>
+        <f xml:space="preserve"> (6*B28 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F28" s="4">
         <v>1400000</v>
@@ -8968,11 +8973,11 @@
         <v>1600000</v>
       </c>
       <c r="C29" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D29" s="1">
-        <f xml:space="preserve"> (4*B29 + 4)*C19</f>
-        <v>1.5999850001499939E-2</v>
+        <f xml:space="preserve"> (6*B29 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F29" s="4">
         <v>1600000</v>
@@ -8990,11 +8995,11 @@
         <v>1800000</v>
       </c>
       <c r="C30" s="1">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
-        <f xml:space="preserve"> (4*B30 + 4)*C19</f>
-        <v>1.799983000169993E-2</v>
+        <f xml:space="preserve"> (6*B30 + 9)*C19</f>
+        <v>0</v>
       </c>
       <c r="F30" s="4">
         <v>1800000</v>
@@ -9011,9 +9016,8 @@
       <c r="B34" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="2">
-        <f xml:space="preserve"> 0.001/LOG(1800000)</f>
-        <v>1.5986513763935291E-4</v>
+      <c r="C34" s="3">
+        <v>0</v>
       </c>
       <c r="F34" t="s">
         <v>3</v>
@@ -9051,7 +9055,7 @@
       </c>
       <c r="D37" s="5">
         <f xml:space="preserve"> LOG(B37)*C34</f>
-        <v>7.9932568819676459E-4</v>
+        <v>0</v>
       </c>
       <c r="F37" s="4">
         <v>100000</v>
@@ -9073,7 +9077,7 @@
       </c>
       <c r="D38" s="5">
         <f>LOG(B38)*C34</f>
-        <v>8.4744988988716072E-4</v>
+        <v>0</v>
       </c>
       <c r="F38" s="4">
         <v>200000</v>
@@ -9095,7 +9099,7 @@
       </c>
       <c r="D39" s="5">
         <f xml:space="preserve"> LOG(B39)*C34</f>
-        <v>8.9557409157755685E-4</v>
+        <v>0</v>
       </c>
       <c r="F39" s="4">
         <v>400000</v>
@@ -9117,7 +9121,7 @@
       </c>
       <c r="D40" s="5">
         <f xml:space="preserve"> LOG(B40)*C34</f>
-        <v>9.2372494494358031E-4</v>
+        <v>0</v>
       </c>
       <c r="F40" s="4">
         <v>600000</v>
@@ -9139,7 +9143,7 @@
       </c>
       <c r="D41" s="5">
         <f xml:space="preserve"> LOG(B41)*C34</f>
-        <v>9.4369829326795308E-4</v>
+        <v>0</v>
       </c>
       <c r="F41" s="4">
         <v>800000</v>
@@ -9161,7 +9165,7 @@
       </c>
       <c r="D42" s="5">
         <f xml:space="preserve"> LOG(B42)*C34</f>
-        <v>9.7184914663397644E-4</v>
+        <v>0</v>
       </c>
       <c r="F42" s="4">
         <v>1200000</v>
@@ -9183,7 +9187,7 @@
       </c>
       <c r="D43" s="5">
         <f xml:space="preserve"> LOG(B43)*C34</f>
-        <v>9.8255160437278719E-4</v>
+        <v>0</v>
       </c>
       <c r="F43" s="4">
         <v>1400000</v>
@@ -9205,7 +9209,7 @@
       </c>
       <c r="D44" s="5">
         <f xml:space="preserve"> LOG(B44)*C34</f>
-        <v>9.9182249495834932E-4</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4">
         <v>1600000</v>
@@ -9223,11 +9227,11 @@
         <v>1800000</v>
       </c>
       <c r="C45" s="5">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="D45" s="5">
         <f xml:space="preserve"> LOG(B45)*C34</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4">
         <v>1800000</v>
@@ -9262,10 +9266,10 @@
         <v>1E-3</v>
       </c>
       <c r="D51" s="1">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="E51" s="5">
-        <v>8.0000000000000004E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -9276,10 +9280,10 @@
         <v>2E-3</v>
       </c>
       <c r="D52" s="1">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="E52" s="5">
-        <v>8.4999999999999995E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -9290,10 +9294,10 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D53" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E53" s="5">
-        <v>8.9999999999999998E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -9304,10 +9308,10 @@
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D54" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E54" s="5">
-        <v>9.2000000000000003E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -9318,10 +9322,10 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D55" s="1">
-        <v>8.0000000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="E55" s="5">
-        <v>9.3999999999999997E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -9332,10 +9336,10 @@
         <v>1.2E-2</v>
       </c>
       <c r="D56" s="1">
-        <v>1.2E-2</v>
+        <v>0</v>
       </c>
       <c r="E56" s="5">
-        <v>9.7000000000000005E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -9346,10 +9350,10 @@
         <v>1.4E-2</v>
       </c>
       <c r="D57" s="1">
-        <v>1.4E-2</v>
+        <v>0</v>
       </c>
       <c r="E57" s="5">
-        <v>9.7999999999999997E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -9360,10 +9364,10 @@
         <v>1.6E-2</v>
       </c>
       <c r="D58" s="1">
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
       <c r="E58" s="5">
-        <v>9.8999999999999999E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -9374,10 +9378,10 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D59" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E59" s="5">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring : Algorithme 2 [Search Min & Max]
</commit_message>
<xml_diff>
--- a/TP2 Search/TP2 Complexity.xlsx
+++ b/TP2 Search/TP2 Complexity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IL\complexity\advanced-algorithmics-and-complexity\TP2 Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBFF7A8-68E5-4B98-A912-F803B63521D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8127D4-FC37-4A46-8243-802606B932D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16D324BE-EF6A-412D-8845-EBC60A736D46}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
   <si>
     <t>N</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Theory 3</t>
+  </si>
+  <si>
+    <t>Texp 1</t>
+  </si>
+  <si>
+    <t>Texp 2</t>
   </si>
 </sst>
 </file>
@@ -8540,10 +8546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AFFE7-F229-43C6-BA9F-9CAF56C460D3}">
-  <dimension ref="B3:H59"/>
+  <dimension ref="B3:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9384,6 +9390,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="4">
+        <v>100000</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B73" s="4">
+        <v>200000</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="4">
+        <v>400000</v>
+      </c>
+      <c r="C74" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="4">
+        <v>600000</v>
+      </c>
+      <c r="C75" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D75" s="1">
+        <v>0</v>
+      </c>
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B76" s="4">
+        <v>800000</v>
+      </c>
+      <c r="C76" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D76" s="1">
+        <v>0</v>
+      </c>
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="4">
+        <v>1200000</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>0</v>
+      </c>
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="4">
+        <v>1400000</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D78" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="4">
+        <v>1600000</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>1800000</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E80" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactoring : TP 2
</commit_message>
<xml_diff>
--- a/TP2 Search/TP2 Complexity.xlsx
+++ b/TP2 Search/TP2 Complexity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IL\complexity\advanced-algorithmics-and-complexity\TP2 Search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8127D4-FC37-4A46-8243-802606B932D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCF4AD0-4EED-488B-95D1-102A05B7BA6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{16D324BE-EF6A-412D-8845-EBC60A736D46}"/>
   </bookViews>
@@ -3858,6 +3858,532 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="487418752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-DZ"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-DZ"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Pire cas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-DZ"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$B$72:$B$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$C$72:$C$80</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC16-4F34-BF07-212EAA581AF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$B$72:$B$80</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$D$72:$D$80</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CC16-4F34-BF07-212EAA581AF0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="478151392"/>
+        <c:axId val="478152048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="478151392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-DZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478152048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="478152048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-DZ"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="478151392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4226,6 +4752,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -7455,6 +8021,544 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8033,15 +9137,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8105,15 +9209,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>552449</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>685801</xdr:colOff>
+      <xdr:colOff>504826</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8177,15 +9281,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:colOff>238126</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8212,16 +9316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8241,6 +9345,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B081707E-2430-4675-A7FB-DF423E57166E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8548,8 +9688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3AFFE7-F229-43C6-BA9F-9CAF56C460D3}">
   <dimension ref="B3:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9481,7 +10621,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="D78" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="E78" s="5"/>
     </row>
@@ -9490,7 +10630,7 @@
         <v>1600000</v>
       </c>
       <c r="C79" s="1">
-        <v>1.2E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D79" s="1">
         <v>1.4999999999999999E-2</v>
@@ -9502,7 +10642,7 @@
         <v>1800000</v>
       </c>
       <c r="C80" s="1">
-        <v>1.6E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D80" s="1">
         <v>1.4999999999999999E-2</v>

</xml_diff>